<commit_message>
Update edited session - 2025-09-19T00:21:11.734Z - Cache Bust ID: 1758241271734yfegd7oe4
</commit_message>
<xml_diff>
--- a/log_history/Y4_B2526_Dermatology_checklist1758240841195_415554c8d435e0c6f15eae4c6d0a20d4db600edb4f28068e43dd237ba5e41fec.xlsx
+++ b/log_history/Y4_B2526_Dermatology_checklist1758240841195_415554c8d435e0c6f15eae4c6d0a20d4db600edb4f28068e43dd237ba5e41fec.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Dermatology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:F57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -464,7 +464,7 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>210306</v>
+        <v>210319</v>
       </c>
       <c r="B4" t="str">
         <v>Dermatology</v>
@@ -473,7 +473,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D4" t="str">
-        <v>03:14:25</v>
+        <v>03:14:26</v>
       </c>
       <c r="E4" t="str">
         <v>Scan</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>210319</v>
+        <v>210334</v>
       </c>
       <c r="B5" t="str">
         <v>Dermatology</v>
@@ -493,7 +493,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D5" t="str">
-        <v>03:14:26</v>
+        <v>03:14:30</v>
       </c>
       <c r="E5" t="str">
         <v>Scan</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>210333</v>
+        <v>210340</v>
       </c>
       <c r="B6" t="str">
         <v>Dermatology</v>
@@ -513,7 +513,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D6" t="str">
-        <v>03:14:29</v>
+        <v>03:14:31</v>
       </c>
       <c r="E6" t="str">
         <v>Scan</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>210334</v>
+        <v>210385</v>
       </c>
       <c r="B7" t="str">
         <v>Dermatology</v>
@@ -533,7 +533,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D7" t="str">
-        <v>03:14:30</v>
+        <v>03:14:32</v>
       </c>
       <c r="E7" t="str">
         <v>Scan</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>210340</v>
+        <v>210387</v>
       </c>
       <c r="B8" t="str">
         <v>Dermatology</v>
@@ -553,7 +553,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D8" t="str">
-        <v>03:14:31</v>
+        <v>03:14:33</v>
       </c>
       <c r="E8" t="str">
         <v>Scan</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>210385</v>
+        <v>210421</v>
       </c>
       <c r="B9" t="str">
         <v>Dermatology</v>
@@ -573,7 +573,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D9" t="str">
-        <v>03:14:32</v>
+        <v>03:14:35</v>
       </c>
       <c r="E9" t="str">
         <v>Scan</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>210387</v>
+        <v>210435</v>
       </c>
       <c r="B10" t="str">
         <v>Dermatology</v>
@@ -593,7 +593,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D10" t="str">
-        <v>03:14:33</v>
+        <v>03:14:36</v>
       </c>
       <c r="E10" t="str">
         <v>Scan</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>210401</v>
+        <v>210438</v>
       </c>
       <c r="B11" t="str">
         <v>Dermatology</v>
@@ -613,7 +613,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D11" t="str">
-        <v>03:14:34</v>
+        <v>03:14:38</v>
       </c>
       <c r="E11" t="str">
         <v>Scan</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>210421</v>
+        <v>210509</v>
       </c>
       <c r="B12" t="str">
         <v>Dermatology</v>
@@ -633,7 +633,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D12" t="str">
-        <v>03:14:35</v>
+        <v>03:14:38</v>
       </c>
       <c r="E12" t="str">
         <v>Scan</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>210435</v>
+        <v>210513</v>
       </c>
       <c r="B13" t="str">
         <v>Dermatology</v>
@@ -653,7 +653,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D13" t="str">
-        <v>03:14:36</v>
+        <v>03:14:40</v>
       </c>
       <c r="E13" t="str">
         <v>Scan</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>210438</v>
+        <v>210516</v>
       </c>
       <c r="B14" t="str">
         <v>Dermatology</v>
@@ -673,7 +673,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D14" t="str">
-        <v>03:14:38</v>
+        <v>03:14:40</v>
       </c>
       <c r="E14" t="str">
         <v>Scan</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>210509</v>
+        <v>210558</v>
       </c>
       <c r="B15" t="str">
         <v>Dermatology</v>
@@ -693,7 +693,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D15" t="str">
-        <v>03:14:38</v>
+        <v>03:14:42</v>
       </c>
       <c r="E15" t="str">
         <v>Scan</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>210513</v>
+        <v>210621</v>
       </c>
       <c r="B16" t="str">
         <v>Dermatology</v>
@@ -713,7 +713,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D16" t="str">
-        <v>03:14:40</v>
+        <v>03:14:43</v>
       </c>
       <c r="E16" t="str">
         <v>Scan</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>210516</v>
+        <v>210686</v>
       </c>
       <c r="B17" t="str">
         <v>Dermatology</v>
@@ -733,7 +733,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>03:14:40</v>
+        <v>03:14:44</v>
       </c>
       <c r="E17" t="str">
         <v>Scan</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>210558</v>
+        <v>210703</v>
       </c>
       <c r="B18" t="str">
         <v>Dermatology</v>
@@ -753,7 +753,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>03:14:42</v>
+        <v>03:14:45</v>
       </c>
       <c r="E18" t="str">
         <v>Scan</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>210621</v>
+        <v>210727</v>
       </c>
       <c r="B19" t="str">
         <v>Dermatology</v>
@@ -773,7 +773,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>03:14:43</v>
+        <v>03:14:46</v>
       </c>
       <c r="E19" t="str">
         <v>Scan</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>210686</v>
+        <v>210762</v>
       </c>
       <c r="B20" t="str">
         <v>Dermatology</v>
@@ -793,7 +793,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>03:14:44</v>
+        <v>03:14:47</v>
       </c>
       <c r="E20" t="str">
         <v>Scan</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>210703</v>
+        <v>210809</v>
       </c>
       <c r="B21" t="str">
         <v>Dermatology</v>
@@ -813,7 +813,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>03:14:45</v>
+        <v>03:14:48</v>
       </c>
       <c r="E21" t="str">
         <v>Scan</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>210727</v>
+        <v>210799</v>
       </c>
       <c r="B22" t="str">
         <v>Dermatology</v>
@@ -833,7 +833,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>03:14:46</v>
+        <v>03:14:49</v>
       </c>
       <c r="E22" t="str">
         <v>Scan</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>210762</v>
+        <v>210828</v>
       </c>
       <c r="B23" t="str">
         <v>Dermatology</v>
@@ -853,7 +853,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>03:14:47</v>
+        <v>03:14:50</v>
       </c>
       <c r="E23" t="str">
         <v>Scan</v>
@@ -864,7 +864,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>210809</v>
+        <v>210832</v>
       </c>
       <c r="B24" t="str">
         <v>Dermatology</v>
@@ -873,7 +873,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D24" t="str">
-        <v>03:14:48</v>
+        <v>03:14:51</v>
       </c>
       <c r="E24" t="str">
         <v>Scan</v>
@@ -884,7 +884,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>210799</v>
+        <v>210836</v>
       </c>
       <c r="B25" t="str">
         <v>Dermatology</v>
@@ -893,7 +893,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D25" t="str">
-        <v>03:14:49</v>
+        <v>03:14:52</v>
       </c>
       <c r="E25" t="str">
         <v>Scan</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>210828</v>
+        <v>210839</v>
       </c>
       <c r="B26" t="str">
         <v>Dermatology</v>
@@ -913,7 +913,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D26" t="str">
-        <v>03:14:50</v>
+        <v>03:14:53</v>
       </c>
       <c r="E26" t="str">
         <v>Scan</v>
@@ -924,7 +924,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>210832</v>
+        <v>210858</v>
       </c>
       <c r="B27" t="str">
         <v>Dermatology</v>
@@ -933,7 +933,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D27" t="str">
-        <v>03:14:51</v>
+        <v>03:14:54</v>
       </c>
       <c r="E27" t="str">
         <v>Scan</v>
@@ -944,7 +944,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>210836</v>
+        <v>210887</v>
       </c>
       <c r="B28" t="str">
         <v>Dermatology</v>
@@ -953,7 +953,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D28" t="str">
-        <v>03:14:52</v>
+        <v>03:15:01</v>
       </c>
       <c r="E28" t="str">
         <v>Scan</v>
@@ -964,7 +964,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>210839</v>
+        <v>210892</v>
       </c>
       <c r="B29" t="str">
         <v>Dermatology</v>
@@ -973,7 +973,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D29" t="str">
-        <v>03:14:53</v>
+        <v>03:15:02</v>
       </c>
       <c r="E29" t="str">
         <v>Scan</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>210858</v>
+        <v>210902</v>
       </c>
       <c r="B30" t="str">
         <v>Dermatology</v>
@@ -993,7 +993,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D30" t="str">
-        <v>03:14:54</v>
+        <v>03:15:03</v>
       </c>
       <c r="E30" t="str">
         <v>Scan</v>
@@ -1004,7 +1004,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>210887</v>
+        <v>210905</v>
       </c>
       <c r="B31" t="str">
         <v>Dermatology</v>
@@ -1013,7 +1013,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D31" t="str">
-        <v>03:15:01</v>
+        <v>03:15:04</v>
       </c>
       <c r="E31" t="str">
         <v>Scan</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>210892</v>
+        <v>210910</v>
       </c>
       <c r="B32" t="str">
         <v>Dermatology</v>
@@ -1033,7 +1033,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D32" t="str">
-        <v>03:15:02</v>
+        <v>03:15:05</v>
       </c>
       <c r="E32" t="str">
         <v>Scan</v>
@@ -1044,7 +1044,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>210902</v>
+        <v>210921</v>
       </c>
       <c r="B33" t="str">
         <v>Dermatology</v>
@@ -1053,7 +1053,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D33" t="str">
-        <v>03:15:03</v>
+        <v>03:15:07</v>
       </c>
       <c r="E33" t="str">
         <v>Scan</v>
@@ -1064,7 +1064,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>210905</v>
+        <v>210927</v>
       </c>
       <c r="B34" t="str">
         <v>Dermatology</v>
@@ -1073,7 +1073,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D34" t="str">
-        <v>03:15:04</v>
+        <v>03:15:08</v>
       </c>
       <c r="E34" t="str">
         <v>Scan</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>210910</v>
+        <v>210939</v>
       </c>
       <c r="B35" t="str">
         <v>Dermatology</v>
@@ -1093,7 +1093,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D35" t="str">
-        <v>03:15:05</v>
+        <v>03:15:09</v>
       </c>
       <c r="E35" t="str">
         <v>Scan</v>
@@ -1104,7 +1104,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>210921</v>
+        <v>210941</v>
       </c>
       <c r="B36" t="str">
         <v>Dermatology</v>
@@ -1113,7 +1113,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D36" t="str">
-        <v>03:15:07</v>
+        <v>03:15:11</v>
       </c>
       <c r="E36" t="str">
         <v>Scan</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>210927</v>
+        <v>210947</v>
       </c>
       <c r="B37" t="str">
         <v>Dermatology</v>
@@ -1133,7 +1133,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D37" t="str">
-        <v>03:15:08</v>
+        <v>03:15:12</v>
       </c>
       <c r="E37" t="str">
         <v>Scan</v>
@@ -1144,7 +1144,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>210939</v>
+        <v>210965</v>
       </c>
       <c r="B38" t="str">
         <v>Dermatology</v>
@@ -1153,7 +1153,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D38" t="str">
-        <v>03:15:09</v>
+        <v>03:15:13</v>
       </c>
       <c r="E38" t="str">
         <v>Scan</v>
@@ -1164,7 +1164,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>210941</v>
+        <v>210994</v>
       </c>
       <c r="B39" t="str">
         <v>Dermatology</v>
@@ -1173,7 +1173,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D39" t="str">
-        <v>03:15:11</v>
+        <v>03:15:20</v>
       </c>
       <c r="E39" t="str">
         <v>Scan</v>
@@ -1184,7 +1184,7 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>210947</v>
+        <v>211002</v>
       </c>
       <c r="B40" t="str">
         <v>Dermatology</v>
@@ -1193,7 +1193,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D40" t="str">
-        <v>03:15:12</v>
+        <v>03:15:21</v>
       </c>
       <c r="E40" t="str">
         <v>Scan</v>
@@ -1204,7 +1204,7 @@
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>210965</v>
+        <v>211003</v>
       </c>
       <c r="B41" t="str">
         <v>Dermatology</v>
@@ -1213,7 +1213,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D41" t="str">
-        <v>03:15:13</v>
+        <v>03:15:23</v>
       </c>
       <c r="E41" t="str">
         <v>Scan</v>
@@ -1224,7 +1224,7 @@
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>210994</v>
+        <v>211024</v>
       </c>
       <c r="B42" t="str">
         <v>Dermatology</v>
@@ -1233,7 +1233,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D42" t="str">
-        <v>03:15:20</v>
+        <v>03:15:24</v>
       </c>
       <c r="E42" t="str">
         <v>Scan</v>
@@ -1244,7 +1244,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>211002</v>
+        <v>211025</v>
       </c>
       <c r="B43" t="str">
         <v>Dermatology</v>
@@ -1253,7 +1253,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D43" t="str">
-        <v>03:15:21</v>
+        <v>03:15:25</v>
       </c>
       <c r="E43" t="str">
         <v>Scan</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>211003</v>
+        <v>211029</v>
       </c>
       <c r="B44" t="str">
         <v>Dermatology</v>
@@ -1273,7 +1273,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D44" t="str">
-        <v>03:15:23</v>
+        <v>03:15:26</v>
       </c>
       <c r="E44" t="str">
         <v>Scan</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>211024</v>
+        <v>211044</v>
       </c>
       <c r="B45" t="str">
         <v>Dermatology</v>
@@ -1293,7 +1293,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D45" t="str">
-        <v>03:15:24</v>
+        <v>03:15:28</v>
       </c>
       <c r="E45" t="str">
         <v>Scan</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>211025</v>
+        <v>211048</v>
       </c>
       <c r="B46" t="str">
         <v>Dermatology</v>
@@ -1313,7 +1313,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D46" t="str">
-        <v>03:15:25</v>
+        <v>03:15:29</v>
       </c>
       <c r="E46" t="str">
         <v>Scan</v>
@@ -1324,7 +1324,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>211029</v>
+        <v>211056</v>
       </c>
       <c r="B47" t="str">
         <v>Dermatology</v>
@@ -1333,7 +1333,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D47" t="str">
-        <v>03:15:26</v>
+        <v>03:15:31</v>
       </c>
       <c r="E47" t="str">
         <v>Scan</v>
@@ -1344,7 +1344,7 @@
     </row>
     <row r="48">
       <c r="A48" t="str">
-        <v>211044</v>
+        <v>211060</v>
       </c>
       <c r="B48" t="str">
         <v>Dermatology</v>
@@ -1353,7 +1353,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D48" t="str">
-        <v>03:15:28</v>
+        <v>03:15:32</v>
       </c>
       <c r="E48" t="str">
         <v>Scan</v>
@@ -1364,7 +1364,7 @@
     </row>
     <row r="49">
       <c r="A49" t="str">
-        <v>211048</v>
+        <v>211063</v>
       </c>
       <c r="B49" t="str">
         <v>Dermatology</v>
@@ -1373,7 +1373,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D49" t="str">
-        <v>03:15:29</v>
+        <v>03:15:33</v>
       </c>
       <c r="E49" t="str">
         <v>Scan</v>
@@ -1384,7 +1384,7 @@
     </row>
     <row r="50">
       <c r="A50" t="str">
-        <v>211056</v>
+        <v>211069</v>
       </c>
       <c r="B50" t="str">
         <v>Dermatology</v>
@@ -1393,7 +1393,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D50" t="str">
-        <v>03:15:31</v>
+        <v>03:15:34</v>
       </c>
       <c r="E50" t="str">
         <v>Scan</v>
@@ -1404,7 +1404,7 @@
     </row>
     <row r="51">
       <c r="A51" t="str">
-        <v>211060</v>
+        <v>211073</v>
       </c>
       <c r="B51" t="str">
         <v>Dermatology</v>
@@ -1413,7 +1413,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D51" t="str">
-        <v>03:15:32</v>
+        <v>03:15:35</v>
       </c>
       <c r="E51" t="str">
         <v>Scan</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="52">
       <c r="A52" t="str">
-        <v>211063</v>
+        <v>211934</v>
       </c>
       <c r="B52" t="str">
         <v>Dermatology</v>
@@ -1433,7 +1433,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D52" t="str">
-        <v>03:15:33</v>
+        <v>03:15:37</v>
       </c>
       <c r="E52" t="str">
         <v>Scan</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="53">
       <c r="A53" t="str">
-        <v>211069</v>
+        <v>220467</v>
       </c>
       <c r="B53" t="str">
         <v>Dermatology</v>
@@ -1453,7 +1453,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D53" t="str">
-        <v>03:15:34</v>
+        <v>03:15:38</v>
       </c>
       <c r="E53" t="str">
         <v>Scan</v>
@@ -1464,7 +1464,7 @@
     </row>
     <row r="54">
       <c r="A54" t="str">
-        <v>211073</v>
+        <v>221082</v>
       </c>
       <c r="B54" t="str">
         <v>Dermatology</v>
@@ -1473,7 +1473,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D54" t="str">
-        <v>03:15:35</v>
+        <v>03:15:39</v>
       </c>
       <c r="E54" t="str">
         <v>Scan</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="55">
       <c r="A55" t="str">
-        <v>211934</v>
+        <v>221105</v>
       </c>
       <c r="B55" t="str">
         <v>Dermatology</v>
@@ -1493,7 +1493,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D55" t="str">
-        <v>03:15:37</v>
+        <v>03:15:40</v>
       </c>
       <c r="E55" t="str">
         <v>Scan</v>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="56">
       <c r="A56" t="str">
-        <v>220467</v>
+        <v>221142</v>
       </c>
       <c r="B56" t="str">
         <v>Dermatology</v>
@@ -1513,7 +1513,7 @@
         <v>19/09/2025</v>
       </c>
       <c r="D56" t="str">
-        <v>03:15:38</v>
+        <v>03:15:41</v>
       </c>
       <c r="E56" t="str">
         <v>Scan</v>
@@ -1524,7 +1524,7 @@
     </row>
     <row r="57">
       <c r="A57" t="str">
-        <v>221082</v>
+        <v>221155</v>
       </c>
       <c r="B57" t="str">
         <v>Dermatology</v>
@@ -1533,78 +1533,18 @@
         <v>19/09/2025</v>
       </c>
       <c r="D57" t="str">
-        <v>03:15:39</v>
+        <v>03:15:43</v>
       </c>
       <c r="E57" t="str">
         <v>Scan</v>
       </c>
       <c r="F57" t="str">
-        <v>dr.manalsalah99@gmail.com</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="str">
-        <v>221105</v>
-      </c>
-      <c r="B58" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C58" t="str">
-        <v>19/09/2025</v>
-      </c>
-      <c r="D58" t="str">
-        <v>03:15:40</v>
-      </c>
-      <c r="E58" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F58" t="str">
-        <v>dr.manalsalah99@gmail.com</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="str">
-        <v>221142</v>
-      </c>
-      <c r="B59" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C59" t="str">
-        <v>19/09/2025</v>
-      </c>
-      <c r="D59" t="str">
-        <v>03:15:41</v>
-      </c>
-      <c r="E59" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F59" t="str">
-        <v>dr.manalsalah99@gmail.com</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="str">
-        <v>221155</v>
-      </c>
-      <c r="B60" t="str">
-        <v>Dermatology</v>
-      </c>
-      <c r="C60" t="str">
-        <v>19/09/2025</v>
-      </c>
-      <c r="D60" t="str">
-        <v>03:15:43</v>
-      </c>
-      <c r="E60" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F60" t="str">
         <v>dr.manalsalah99@gmail.com</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F60"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F57"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>